<commit_message>
updated forms, tasks and targets
</commit_message>
<xml_diff>
--- a/forms/app/update_summary.xlsx
+++ b/forms/app/update_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -192,7 +192,7 @@
     <t xml:space="preserve">summary</t>
   </si>
   <si>
-    <t xml:space="preserve">Summary</t>
+    <t xml:space="preserve">NO_LABEL</t>
   </si>
   <si>
     <t xml:space="preserve">field-list summary</t>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t xml:space="preserve">Assessment follow up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">update_summary_context</t>
   </si>
   <si>
     <t xml:space="preserve">pages</t>
@@ -718,10 +715,10 @@
   </sheetPr>
   <dimension ref="A1:AP1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="C4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="C6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3951,7 +3948,7 @@
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4007,22 +4004,22 @@
       <c r="Y1" s="41"/>
       <c r="Z1" s="41"/>
     </row>
-    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="43" t="s">
         <v>72</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="C2" s="18" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2020-05-04  17-16</v>
+        <v>2020-05-11  10-34</v>
       </c>
       <c r="D2" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="45" t="s">
         <v>74</v>
-      </c>
-      <c r="E2" s="45" t="s">
-        <v>75</v>
       </c>
       <c r="F2" s="45"/>
       <c r="G2" s="43"/>

</xml_diff>